<commit_message>
updating the supp_tables with renamed SBS1
</commit_message>
<xml_diff>
--- a/supp_data/PCAWG.sig.pathway.significant.interactions.xlsx
+++ b/supp_data/PCAWG.sig.pathway.significant.interactions.xlsx
@@ -38,7 +38,7 @@
     <t xml:space="preserve">TP53</t>
   </si>
   <si>
-    <t xml:space="preserve">Ageing</t>
+    <t xml:space="preserve">CL SBS1</t>
   </si>
   <si>
     <t xml:space="preserve">SBS30</t>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">PI3K</t>
   </si>
   <si>
-    <t xml:space="preserve">SBS5</t>
+    <t xml:space="preserve">CL SBS5</t>
   </si>
   <si>
     <t xml:space="preserve">MYC</t>
@@ -502,7 +502,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0.006</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="4">
@@ -519,7 +519,7 @@
         <v>5</v>
       </c>
       <c r="G4" t="n">
-        <v>0.005</v>
+        <v>0.011</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -582,30 +582,30 @@
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0.006</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-2.51001993219839</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>-1.90088815710587</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H11" t="n">
-        <v>0.015</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0.031</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
@@ -613,25 +613,25 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>-2.51001993219839</v>
       </c>
       <c r="C12" t="n">
-        <v>-1.90088815710587</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>0.029</v>
       </c>
       <c r="I12" t="n">
-        <v>0.038</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
         <v>1</v>
@@ -690,7 +690,7 @@
         <v>11</v>
       </c>
       <c r="G3" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -710,10 +710,10 @@
         <v>18</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00700000000000001</v>
+        <v>0.00900000000000001</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="8">
@@ -758,10 +758,10 @@
         <v>4</v>
       </c>
       <c r="G10" t="n">
-        <v>0.00600000000000001</v>
+        <v>0.00700000000000001</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="11">
@@ -778,7 +778,7 @@
         <v>11</v>
       </c>
       <c r="G11" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
@@ -798,10 +798,10 @@
         <v>18</v>
       </c>
       <c r="G12" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
       <c r="H12" t="n">
-        <v>0.01</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="16">
@@ -855,13 +855,13 @@
         <v>4</v>
       </c>
       <c r="H18" t="n">
-        <v>0.00600000000000001</v>
+        <v>0.00700000000000001</v>
       </c>
       <c r="I18" t="n">
         <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="19">
@@ -881,7 +881,7 @@
         <v>11</v>
       </c>
       <c r="H19" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
         <v>1</v>
@@ -907,13 +907,13 @@
         <v>18</v>
       </c>
       <c r="H20" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
       <c r="I20" t="n">
-        <v>0.027</v>
+        <v>0.041</v>
       </c>
       <c r="J20" t="n">
-        <v>0.01</v>
+        <v>0.015</v>
       </c>
     </row>
   </sheetData>
@@ -957,82 +957,82 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>2.60309300495891</v>
       </c>
       <c r="C3" t="n">
-        <v>-4.2746883155441</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>0.003</v>
       </c>
       <c r="H3" t="n">
-        <v>0.024</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>2.60309300495891</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>-4.2746883155441</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
-        <v>0.005</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>-3.34065186563383</v>
+        <v>-4.2746883155441</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0.015</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>-4.2746883155441</v>
+        <v>-3.34065186563383</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>0.033</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="10">
@@ -1071,25 +1071,25 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>1.37379431310296</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>0.263766146128955</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="H12" t="n">
-        <v>0.001</v>
+        <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0.013</v>
       </c>
       <c r="J12" t="n">
         <v>1</v>
@@ -1097,25 +1097,25 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1.37379431310296</v>
       </c>
       <c r="C13" t="n">
-        <v>0.263766146128955</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="H13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>0.012</v>
+        <v>1</v>
       </c>
       <c r="J13" t="n">
         <v>1</v>
@@ -1123,77 +1123,77 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1.38974444189436</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.366100106199248</v>
+        <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H14" t="n">
-        <v>1</v>
+        <v>0.012</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>0.004</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0.272471984446401</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>-0.366100106199248</v>
       </c>
       <c r="G15" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H15" t="n">
         <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>0.026</v>
+        <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>1</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B16" t="n">
-        <v>1.38974444189436</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>0.272471984446401</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H16" t="n">
-        <v>0.00600000000000001</v>
+        <v>1</v>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0.026</v>
       </c>
       <c r="J16" t="n">
         <v>1</v>
@@ -1235,25 +1235,25 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B22" t="n">
-        <v>1.32338568758481</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>2.15229845369274</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="H22" t="n">
-        <v>0.001</v>
+        <v>1</v>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0.013</v>
       </c>
       <c r="J22" t="n">
         <v>1</v>
@@ -1261,25 +1261,25 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>1.32338568758481</v>
       </c>
       <c r="C23" t="n">
-        <v>2.15229845369274</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="H23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>0.012</v>
+        <v>1</v>
       </c>
       <c r="J23" t="n">
         <v>1</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B24" t="n">
         <v>0</v>
@@ -1296,10 +1296,10 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-3.30071537648484</v>
+        <v>-1.50816185953598</v>
       </c>
       <c r="G24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H24" t="n">
         <v>1</v>
@@ -1308,59 +1308,59 @@
         <v>1</v>
       </c>
       <c r="J24" t="n">
-        <v>0.004</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>2.06167151156894</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-2.20608949687461</v>
+        <v>-3.30071537648484</v>
       </c>
       <c r="G25" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H25" t="n">
         <v>1</v>
       </c>
       <c r="I25" t="n">
-        <v>0.026</v>
+        <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>0.026</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B26" t="n">
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>2.06167151156894</v>
       </c>
       <c r="D26" t="n">
-        <v>-1.50816185953598</v>
+        <v>-2.20608949687461</v>
       </c>
       <c r="G26" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H26" t="n">
         <v>1</v>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0.026</v>
       </c>
       <c r="J26" t="n">
-        <v>0.031</v>
+        <v>0.033</v>
       </c>
     </row>
   </sheetData>
@@ -1410,77 +1410,77 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>-6.8690392593615</v>
       </c>
       <c r="D3" t="n">
-        <v>1.39212178194758</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0.018</v>
       </c>
       <c r="J3" t="n">
-        <v>0.002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" t="n">
-        <v>1.15696473061178</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1.39212178194758</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
         <v>0.003</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1.15696473061178</v>
       </c>
       <c r="C5" t="n">
-        <v>-6.8690392593615</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>0.017</v>
       </c>
       <c r="I5" t="n">
-        <v>0.024</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
         <v>1</v>
@@ -1531,7 +1531,7 @@
         <v>0.004</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="12">
@@ -1551,7 +1551,7 @@
         <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
     </row>
     <row r="13">
@@ -1568,7 +1568,7 @@
         <v>18</v>
       </c>
       <c r="G13" t="n">
-        <v>0.003</v>
+        <v>0.012</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
@@ -1619,7 +1619,7 @@
         <v>0.004</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="20">
@@ -1639,7 +1639,7 @@
         <v>1</v>
       </c>
       <c r="H20" t="n">
-        <v>0.05</v>
+        <v>0.038</v>
       </c>
     </row>
     <row r="21">
@@ -1659,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="H21" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
     </row>
     <row r="22">
@@ -1679,7 +1679,7 @@
         <v>1</v>
       </c>
       <c r="H22" t="n">
-        <v>0.026</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="23">
@@ -1696,7 +1696,7 @@
         <v>18</v>
       </c>
       <c r="G23" t="n">
-        <v>0.003</v>
+        <v>0.012</v>
       </c>
       <c r="H23" t="n">
         <v>1</v>
@@ -1776,7 +1776,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.004</v>
+        <v>0.00600000000000001</v>
       </c>
       <c r="K3" t="n">
         <v>1</v>
@@ -1805,7 +1805,7 @@
         <v>32</v>
       </c>
       <c r="I4" t="n">
-        <v>0.00600000000000001</v>
+        <v>0.003</v>
       </c>
       <c r="J4" t="n">
         <v>1</v>
@@ -1814,7 +1814,7 @@
         <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>0.016</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="5">
@@ -1840,13 +1840,13 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>0.005</v>
+        <v>0.00800000000000001</v>
       </c>
       <c r="K5" t="n">
-        <v>0.001</v>
+        <v>0.004</v>
       </c>
       <c r="L5" t="n">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="6">
@@ -1878,7 +1878,7 @@
         <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
     </row>
     <row r="10">
@@ -1941,10 +1941,10 @@
         <v>13</v>
       </c>
       <c r="I12" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="J12" t="n">
-        <v>0.003</v>
+        <v>0.00600000000000001</v>
       </c>
       <c r="K12" t="n">
         <v>1</v>
@@ -1982,7 +1982,7 @@
         <v>1</v>
       </c>
       <c r="L13" t="n">
-        <v>0.005</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="14">
@@ -2008,13 +2008,13 @@
         <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>0.00900000000000001</v>
+        <v>0.00800000000000001</v>
       </c>
       <c r="K14" t="n">
         <v>0.002</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="15">
@@ -2037,7 +2037,7 @@
         <v>33</v>
       </c>
       <c r="I15" t="n">
-        <v>0.009</v>
+        <v>0.011</v>
       </c>
       <c r="J15" t="n">
         <v>1</v>
@@ -2046,7 +2046,7 @@
         <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
     </row>
     <row r="19">
@@ -2091,13 +2091,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B21" t="n">
-        <v>3.05117756976441</v>
+        <v>4.39893020125887</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>2.65565078317008</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -2106,13 +2106,13 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="I21" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="J21" t="n">
-        <v>1</v>
+        <v>0.00600000000000001</v>
       </c>
       <c r="K21" t="n">
         <v>1</v>
@@ -2123,13 +2123,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B22" t="n">
-        <v>4.39893020125887</v>
+        <v>3.05117756976441</v>
       </c>
       <c r="C22" t="n">
-        <v>2.65565078317008</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -2138,13 +2138,13 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="I22" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="J22" t="n">
-        <v>0.003</v>
+        <v>1</v>
       </c>
       <c r="K22" t="n">
         <v>1</v>
@@ -2173,7 +2173,7 @@
         <v>32</v>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0.029</v>
       </c>
       <c r="J23" t="n">
         <v>1</v>
@@ -2182,7 +2182,7 @@
         <v>1</v>
       </c>
       <c r="L23" t="n">
-        <v>0.005</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="24">
@@ -2208,13 +2208,13 @@
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>0.00900000000000001</v>
+        <v>0.00800000000000001</v>
       </c>
       <c r="K24" t="n">
         <v>0.002</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="25">
@@ -2237,7 +2237,7 @@
         <v>33</v>
       </c>
       <c r="I25" t="n">
-        <v>0.009</v>
+        <v>0.011</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>
@@ -2246,7 +2246,7 @@
         <v>0.015</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
     </row>
   </sheetData>
@@ -2311,7 +2311,7 @@
         <v>11</v>
       </c>
       <c r="H3" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -2368,89 +2368,89 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B9" t="n">
-        <v>1.36460690044162</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>2.14105637438993</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>-1.29071485723344</v>
+        <v>0.225550684000814</v>
       </c>
       <c r="F9" t="n">
-        <v>1.22047117445816</v>
+        <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="J9" t="n">
-        <v>0.00600000000000001</v>
+        <v>1</v>
       </c>
       <c r="K9" t="n">
         <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>0.002</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>0.004</v>
+        <v>0.00900000000000001</v>
       </c>
       <c r="N9" t="n">
-        <v>0.00600000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1.36460690044162</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>2.14105637438993</v>
       </c>
       <c r="E10" t="n">
-        <v>0.225550684000814</v>
+        <v>-1.29071485723344</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>1.22047117445816</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>0.005</v>
       </c>
       <c r="K10" t="n">
         <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>0.002</v>
       </c>
       <c r="M10" t="n">
-        <v>0.00600000000000001</v>
+        <v>0.007</v>
       </c>
       <c r="N10" t="n">
-        <v>1</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.143759371392738</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.203223331670282</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -2459,16 +2459,16 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.145574319115521</v>
+        <v>0.951480822059076</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J11" t="n">
-        <v>0.004</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>0.002</v>
+        <v>1</v>
       </c>
       <c r="L11" t="n">
         <v>1</v>
@@ -2477,18 +2477,18 @@
         <v>1</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>0.00900000000000001</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.133327182047127</v>
+        <v>0.143759371392738</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>0.203223331670282</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -2497,16 +2497,16 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.145574319115521</v>
       </c>
       <c r="I12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J12" t="n">
-        <v>0.014</v>
+        <v>0.003</v>
       </c>
       <c r="K12" t="n">
-        <v>1</v>
+        <v>0.003</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
@@ -2515,21 +2515,21 @@
         <v>1</v>
       </c>
       <c r="N12" t="n">
-        <v>1</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>0.133327182047127</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.254444229264285</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -2538,16 +2538,16 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>0.017</v>
       </c>
       <c r="K13" t="n">
         <v>1</v>
       </c>
       <c r="L13" t="n">
-        <v>0.042</v>
+        <v>1</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
@@ -2558,7 +2558,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -2567,16 +2567,16 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>0.254444229264285</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.951480822059076</v>
+        <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J14" t="n">
         <v>1</v>
@@ -2585,13 +2585,13 @@
         <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="M14" t="n">
         <v>1</v>
       </c>
       <c r="N14" t="n">
-        <v>0.00800000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -2642,89 +2642,89 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B20" t="n">
-        <v>0.20966283402879</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.363809252589274</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.190600967894006</v>
+        <v>1.11695624060739</v>
       </c>
       <c r="F20" t="n">
-        <v>0.184054973692348</v>
+        <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="J20" t="n">
-        <v>0.00600000000000001</v>
+        <v>1</v>
       </c>
       <c r="K20" t="n">
         <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>0.002</v>
+        <v>1</v>
       </c>
       <c r="M20" t="n">
-        <v>0.004</v>
+        <v>0.00900000000000001</v>
       </c>
       <c r="N20" t="n">
-        <v>0.00600000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>0.20966283402879</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>0.363809252589274</v>
       </c>
       <c r="E21" t="n">
-        <v>1.11695624060739</v>
+        <v>-0.190600967894006</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>0.184054973692348</v>
       </c>
       <c r="I21" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="J21" t="n">
-        <v>1</v>
+        <v>0.005</v>
       </c>
       <c r="K21" t="n">
         <v>1</v>
       </c>
       <c r="L21" t="n">
-        <v>1</v>
+        <v>0.002</v>
       </c>
       <c r="M21" t="n">
-        <v>0.00600000000000001</v>
+        <v>0.007</v>
       </c>
       <c r="N21" t="n">
-        <v>1</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22" t="n">
-        <v>2.20485620123942</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>3.27640141096423</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -2733,16 +2733,16 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>2.14642065892</v>
+        <v>0.227485291230434</v>
       </c>
       <c r="I22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J22" t="n">
-        <v>0.004</v>
+        <v>1</v>
       </c>
       <c r="K22" t="n">
-        <v>0.002</v>
+        <v>1</v>
       </c>
       <c r="L22" t="n">
         <v>1</v>
@@ -2751,18 +2751,18 @@
         <v>1</v>
       </c>
       <c r="N22" t="n">
-        <v>0</v>
+        <v>0.00900000000000001</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B23" t="n">
-        <v>1.32393049586975</v>
+        <v>2.20485620123942</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>3.27640141096423</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -2771,16 +2771,16 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>2.14642065892</v>
       </c>
       <c r="I23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J23" t="n">
-        <v>0.014</v>
+        <v>0.003</v>
       </c>
       <c r="K23" t="n">
-        <v>1</v>
+        <v>0.003</v>
       </c>
       <c r="L23" t="n">
         <v>1</v>
@@ -2789,21 +2789,21 @@
         <v>1</v>
       </c>
       <c r="N23" t="n">
-        <v>1</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>1.32393049586975</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.997369884639188</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -2812,16 +2812,16 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J24" t="n">
-        <v>1</v>
+        <v>0.017</v>
       </c>
       <c r="K24" t="n">
         <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="M24" t="n">
         <v>1</v>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>
@@ -2841,16 +2841,16 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>0.997369884639188</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0.227485291230434</v>
+        <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>
@@ -2859,13 +2859,13 @@
         <v>1</v>
       </c>
       <c r="L25" t="n">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="M25" t="n">
         <v>1</v>
       </c>
       <c r="N25" t="n">
-        <v>0.00800000000000001</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2981,7 +2981,7 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0.005</v>
+        <v>0.00600000000000001</v>
       </c>
       <c r="L9" t="n">
         <v>1</v>
@@ -3039,7 +3039,7 @@
         <v>17</v>
       </c>
       <c r="I11" t="n">
-        <v>0.00800000000000001</v>
+        <v>0.003</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
@@ -3117,7 +3117,7 @@
         <v>1</v>
       </c>
       <c r="K17" t="n">
-        <v>0.005</v>
+        <v>0.00600000000000001</v>
       </c>
       <c r="L17" t="n">
         <v>1</v>
@@ -3181,7 +3181,7 @@
         <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="L19" t="n">
         <v>1</v>
@@ -3207,7 +3207,7 @@
         <v>17</v>
       </c>
       <c r="I20" t="n">
-        <v>0.023</v>
+        <v>0.027</v>
       </c>
       <c r="J20" t="n">
         <v>1</v>
@@ -3284,10 +3284,10 @@
         <v>4</v>
       </c>
       <c r="H3" t="n">
-        <v>0.009</v>
+        <v>0.01</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
@@ -3316,7 +3316,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0.011</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="8">
@@ -3379,13 +3379,13 @@
         <v>4</v>
       </c>
       <c r="I10" t="n">
-        <v>0.009</v>
+        <v>0.01</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
@@ -3420,7 +3420,7 @@
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>0.011</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="12">
@@ -3446,7 +3446,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
         <v>1</v>
@@ -3504,30 +3504,30 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>-3.95948271061582</v>
+        <v>-2.73994552147137</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
-        <v>0.034</v>
+        <v>0.038</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>-2.73994552147137</v>
+        <v>-3.95948271061582</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F5" t="n">
-        <v>0.043</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="9">
@@ -3563,7 +3563,7 @@
         <v>20</v>
       </c>
       <c r="F11" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -3577,7 +3577,7 @@
         <v>18</v>
       </c>
       <c r="F12" t="n">
-        <v>0.028</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="16">
@@ -3613,7 +3613,7 @@
         <v>20</v>
       </c>
       <c r="F18" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -3627,7 +3627,7 @@
         <v>18</v>
       </c>
       <c r="F19" t="n">
-        <v>0.028</v>
+        <v>0.029</v>
       </c>
     </row>
   </sheetData>
@@ -3703,7 +3703,7 @@
         <v>23</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00700000000000001</v>
+        <v>0.001</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -3751,13 +3751,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1.35567240715499</v>
       </c>
       <c r="C10" t="n">
-        <v>0.338839853075239</v>
+        <v>2.18839329118468</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -3766,13 +3766,13 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0.017</v>
       </c>
       <c r="J10" t="n">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
       <c r="K10" t="n">
         <v>1</v>
@@ -3783,39 +3783,39 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.338839853075239</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.184462640753844</v>
+        <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>0.004</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>0.002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -3824,13 +3824,13 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2928976840555</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>-0.184462640753844</v>
       </c>
       <c r="H12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
@@ -3842,36 +3842,36 @@
         <v>1</v>
       </c>
       <c r="L12" t="n">
-        <v>1</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B13" t="n">
-        <v>1.35567240715499</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>2.18839329118468</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>0.2928976840555</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="I13" t="n">
-        <v>0.015</v>
+        <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>0.005</v>
+        <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>1</v>
+        <v>0.041</v>
       </c>
       <c r="L13" t="n">
         <v>1</v>
@@ -3946,7 +3946,7 @@
         <v>20</v>
       </c>
       <c r="J19" t="n">
-        <v>0.019</v>
+        <v>0.032</v>
       </c>
       <c r="K19" t="n">
         <v>1</v>
@@ -3963,37 +3963,37 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>0.287820732003017</v>
       </c>
       <c r="D20" t="n">
-        <v>1.20745885407501</v>
+        <v>0.414564833475857</v>
       </c>
       <c r="E20" t="n">
-        <v>0.466244599503037</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="J20" t="n">
         <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>1</v>
+        <v>0.017</v>
       </c>
       <c r="L20" t="n">
-        <v>0.002</v>
+        <v>0.01</v>
       </c>
       <c r="M20" t="n">
-        <v>0.033</v>
+        <v>1</v>
       </c>
       <c r="N20" t="n">
         <v>1</v>
@@ -4001,7 +4001,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
@@ -4010,16 +4010,16 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>1.20745885407501</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>0.466244599503037</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.901097021895587</v>
+        <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="J21" t="n">
         <v>1</v>
@@ -4028,18 +4028,18 @@
         <v>1</v>
       </c>
       <c r="L21" t="n">
-        <v>1</v>
+        <v>0.003</v>
       </c>
       <c r="M21" t="n">
-        <v>1</v>
+        <v>0.035</v>
       </c>
       <c r="N21" t="n">
-        <v>0.002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -4051,13 +4051,13 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0.526323410532715</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>-0.901097021895587</v>
       </c>
       <c r="I22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J22" t="n">
         <v>1</v>
@@ -4069,45 +4069,45 @@
         <v>1</v>
       </c>
       <c r="M22" t="n">
-        <v>0.049</v>
+        <v>1</v>
       </c>
       <c r="N22" t="n">
-        <v>1</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B23" t="n">
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0.287820732003017</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.414564833475857</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>0.526323410532715</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="J23" t="n">
         <v>1</v>
       </c>
       <c r="K23" t="n">
-        <v>0.015</v>
+        <v>1</v>
       </c>
       <c r="L23" t="n">
-        <v>0.005</v>
+        <v>1</v>
       </c>
       <c r="M23" t="n">
-        <v>1</v>
+        <v>0.043</v>
       </c>
       <c r="N23" t="n">
         <v>1</v>
@@ -4193,19 +4193,19 @@
         <v>27</v>
       </c>
       <c r="J3" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="K3" t="n">
         <v>0.003</v>
       </c>
-      <c r="K3" t="n">
-        <v>0.002</v>
-      </c>
       <c r="L3" t="n">
-        <v>0.025</v>
+        <v>0.023</v>
       </c>
       <c r="M3" t="n">
         <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>0.003</v>
+        <v>0.00700000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -4240,7 +4240,7 @@
         <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="N4" t="n">
         <v>1</v>
@@ -4294,92 +4294,92 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.21789979569767</v>
+        <v>-1.15328861562131</v>
       </c>
       <c r="C10" t="n">
-        <v>0.20457295245258</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1.266570313924</v>
       </c>
       <c r="F10" t="n">
-        <v>0.189949393652309</v>
+        <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="J10" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.017</v>
+        <v>1</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>1</v>
+        <v>0.004</v>
       </c>
       <c r="N10" t="n">
-        <v>0.017</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>0.21789979569767</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.20457295245258</v>
       </c>
       <c r="D11" t="n">
-        <v>0.192342988835529</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.189949393652309</v>
       </c>
       <c r="I11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>0.012</v>
       </c>
       <c r="K11" t="n">
-        <v>1</v>
+        <v>0.015</v>
       </c>
       <c r="L11" t="n">
-        <v>0.023</v>
+        <v>1</v>
       </c>
       <c r="M11" t="n">
         <v>1</v>
       </c>
       <c r="N11" t="n">
-        <v>1</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.148958862235712</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.192342988835529</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -4388,16 +4388,16 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="J12" t="n">
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>0.008</v>
+        <v>1</v>
       </c>
       <c r="L12" t="n">
-        <v>1</v>
+        <v>0.027</v>
       </c>
       <c r="M12" t="n">
         <v>1</v>
@@ -4408,37 +4408,37 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.15328861562131</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>-0.148958862235712</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>1.266570313924</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>1</v>
+        <v>0.009</v>
       </c>
       <c r="L13" t="n">
         <v>1</v>
       </c>
       <c r="M13" t="n">
-        <v>0.005</v>
+        <v>1</v>
       </c>
       <c r="N13" t="n">
         <v>1</v>
@@ -4498,40 +4498,40 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.490037866469666</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.473519332668864</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>-0.822468779075157</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1.51449583324692</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>1.29870961849463</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="K19" t="n">
-        <v>0.013</v>
+        <v>1</v>
       </c>
       <c r="L19" t="n">
-        <v>0.032</v>
+        <v>1</v>
       </c>
       <c r="M19" t="n">
-        <v>1</v>
+        <v>0.002</v>
       </c>
       <c r="N19" t="n">
-        <v>1</v>
+        <v>0.039</v>
       </c>
       <c r="O19" t="n">
         <v>1</v>
@@ -4542,43 +4542,43 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>-0.490037866469666</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>-0.473519332668864</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.822468779075157</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>1.51449583324692</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>1.29870961849463</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="K20" t="n">
-        <v>1</v>
+        <v>0.013</v>
       </c>
       <c r="L20" t="n">
-        <v>1</v>
+        <v>0.028</v>
       </c>
       <c r="M20" t="n">
-        <v>0.008</v>
+        <v>1</v>
       </c>
       <c r="N20" t="n">
-        <v>0.039</v>
+        <v>1</v>
       </c>
       <c r="O20" t="n">
-        <v>0.046</v>
+        <v>1</v>
       </c>
       <c r="P20" t="n">
         <v>1</v>
@@ -4586,13 +4586,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B21" t="n">
-        <v>1.21738012739502</v>
+        <v>-0.761863486217287</v>
       </c>
       <c r="C21" t="n">
-        <v>1.19732018177747</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -4601,19 +4601,19 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>0.885450284534123</v>
       </c>
       <c r="G21" t="n">
-        <v>1.07225449656332</v>
+        <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="K21" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>0.017</v>
+        <v>1</v>
       </c>
       <c r="M21" t="n">
         <v>1</v>
@@ -4622,71 +4622,71 @@
         <v>1</v>
       </c>
       <c r="O21" t="n">
-        <v>1</v>
+        <v>0.004</v>
       </c>
       <c r="P21" t="n">
-        <v>0.017</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>1.21738012739502</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>1.19732018177747</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>2.97506482273952</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>1.07225449656332</v>
       </c>
       <c r="J22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K22" t="n">
-        <v>1</v>
+        <v>0.012</v>
       </c>
       <c r="L22" t="n">
-        <v>1</v>
+        <v>0.015</v>
       </c>
       <c r="M22" t="n">
         <v>1</v>
       </c>
       <c r="N22" t="n">
-        <v>0.023</v>
+        <v>1</v>
       </c>
       <c r="O22" t="n">
         <v>1</v>
       </c>
       <c r="P22" t="n">
-        <v>1</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>-2.39549562558017</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>2.97506482273952</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -4695,19 +4695,19 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="K23" t="n">
         <v>1</v>
       </c>
       <c r="L23" t="n">
-        <v>0.008</v>
+        <v>1</v>
       </c>
       <c r="M23" t="n">
         <v>1</v>
       </c>
       <c r="N23" t="n">
-        <v>1</v>
+        <v>0.027</v>
       </c>
       <c r="O23" t="n">
         <v>1</v>
@@ -4718,13 +4718,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.761863486217287</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>-2.39549562558017</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -4733,19 +4733,19 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.885450284534123</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>1</v>
+        <v>0.009</v>
       </c>
       <c r="M24" t="n">
         <v>1</v>
@@ -4754,7 +4754,7 @@
         <v>1</v>
       </c>
       <c r="O24" t="n">
-        <v>0.005</v>
+        <v>1</v>
       </c>
       <c r="P24" t="n">
         <v>1</v>
@@ -4804,7 +4804,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -4858,10 +4858,10 @@
         <v>4</v>
       </c>
       <c r="H9" t="n">
-        <v>0.017</v>
+        <v>0.01</v>
       </c>
       <c r="I9" t="n">
-        <v>0.008</v>
+        <v>0.013</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -4890,7 +4890,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -4944,10 +4944,10 @@
         <v>4</v>
       </c>
       <c r="H16" t="n">
-        <v>0.017</v>
+        <v>0.01</v>
       </c>
       <c r="I16" t="n">
-        <v>0.008</v>
+        <v>0.013</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -4955,54 +4955,54 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B17" t="n">
-        <v>-2.7158758507827</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-2.73962843570397</v>
+        <v>0.237789529159696</v>
       </c>
       <c r="G17" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="H17" t="n">
-        <v>0.006</v>
+        <v>1</v>
       </c>
       <c r="I17" t="n">
         <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>0.001</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>-2.7158758507827</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.237789529159696</v>
+        <v>-2.73962843570397</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>0.009</v>
       </c>
       <c r="I18" t="n">
         <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>0.024</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5081,7 +5081,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>0.00700000000000001</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="8">
@@ -5135,7 +5135,7 @@
         <v>4</v>
       </c>
       <c r="H10" t="n">
-        <v>0.015</v>
+        <v>0.00600000000000001</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
@@ -5164,7 +5164,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0.004</v>
+        <v>0.012</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
@@ -5247,7 +5247,7 @@
         <v>4</v>
       </c>
       <c r="H18" t="n">
-        <v>0.015</v>
+        <v>0.00600000000000001</v>
       </c>
       <c r="I18" t="n">
         <v>1</v>
@@ -5276,7 +5276,7 @@
         <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>0.004</v>
+        <v>0.012</v>
       </c>
       <c r="J19" t="n">
         <v>1</v>

</xml_diff>